<commit_message>
Automatic sync of changes
</commit_message>
<xml_diff>
--- a/graduate_programs.xlsx
+++ b/graduate_programs.xlsx
@@ -8,24 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\20-29 projects\.github\repositories\graduate_programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9265CDA-4CFB-463E-8ECA-6A4BD05FFD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F177253-14A6-4792-B911-6F6FB32A4C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4520" yWindow="400" windowWidth="14270" windowHeight="4910" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>fields</t>
   </si>
@@ -58,6 +71,78 @@
   </si>
   <si>
     <t>HER analytics</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>university</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>program</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>sent email</t>
+  </si>
+  <si>
+    <t>application deadline</t>
+  </si>
+  <si>
+    <t>funding</t>
+  </si>
+  <si>
+    <t>stipend</t>
+  </si>
+  <si>
+    <t>semester start date</t>
+  </si>
+  <si>
+    <t>Harvard University</t>
+  </si>
+  <si>
+    <t>PhD</t>
+  </si>
+  <si>
+    <t>on-campus</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Columbia University</t>
+  </si>
+  <si>
+    <t>University of Utah</t>
+  </si>
+  <si>
+    <t>hybrid</t>
+  </si>
+  <si>
+    <t>George Mason University</t>
+  </si>
+  <si>
+    <t>full</t>
+  </si>
+  <si>
+    <t>Stanford University</t>
+  </si>
+  <si>
+    <t>yes - waiting for reply</t>
+  </si>
+  <si>
+    <t>Purdue University</t>
+  </si>
+  <si>
+    <t>MSc</t>
+  </si>
+  <si>
+    <t>health sciences</t>
   </si>
 </sst>
 </file>
@@ -104,7 +189,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -400,10 +485,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1"/>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -450,6 +535,205 @@
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBED3AA9-B8C1-469B-B44D-ADE15B706853}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136FD6B1-04F9-4AED-A234-0D06F19ED836}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="2.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2">
+        <v>45962</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>